<commit_message>
Actualizaciones mayo 2019 - Infra
Actualizaciones mayo 2019 - Infra
</commit_message>
<xml_diff>
--- a/proyecto final/Defensa/Infraestructura/Presupuesto.xlsx
+++ b/proyecto final/Defensa/Infraestructura/Presupuesto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20730" windowHeight="11700" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20730" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Presupuesto" sheetId="7" r:id="rId1"/>
@@ -742,54 +742,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -1736,6 +1688,30 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2212,6 +2188,30 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3103,59 +3103,59 @@
   <tableColumns count="8">
     <tableColumn id="1" name="Equipos" dataDxfId="70"/>
     <tableColumn id="2" name="Fabricante" dataDxfId="69"/>
-    <tableColumn id="3" name="Disponibilidad" dataDxfId="1"/>
-    <tableColumn id="5" name="Versión" dataDxfId="68"/>
-    <tableColumn id="6" name="Procesador" dataDxfId="67"/>
-    <tableColumn id="7" name="Utilidad" dataDxfId="66"/>
-    <tableColumn id="8" name="Equipo" dataDxfId="65"/>
-    <tableColumn id="9" name="Replica Tambo 2" dataDxfId="64"/>
+    <tableColumn id="3" name="Disponibilidad" dataDxfId="68"/>
+    <tableColumn id="5" name="Versión" dataDxfId="67"/>
+    <tableColumn id="6" name="Procesador" dataDxfId="66"/>
+    <tableColumn id="7" name="Utilidad" dataDxfId="65"/>
+    <tableColumn id="8" name="Equipo" dataDxfId="64"/>
+    <tableColumn id="9" name="Replica Tambo 2" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A4:H6" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A4:H6" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <autoFilter ref="A4:H6"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Equipos" dataDxfId="61"/>
-    <tableColumn id="2" name="Fabricante" dataDxfId="60"/>
-    <tableColumn id="3" name="Disponibilidad" dataDxfId="59"/>
-    <tableColumn id="5" name="Versión" dataDxfId="58"/>
-    <tableColumn id="6" name="Procesador" dataDxfId="57"/>
-    <tableColumn id="7" name="Utilidad" dataDxfId="56"/>
-    <tableColumn id="8" name="Equipo" dataDxfId="55"/>
-    <tableColumn id="9" name="Contrato privado" dataDxfId="54"/>
+    <tableColumn id="1" name="Equipos" dataDxfId="60"/>
+    <tableColumn id="2" name="Fabricante" dataDxfId="59"/>
+    <tableColumn id="3" name="Disponibilidad" dataDxfId="58"/>
+    <tableColumn id="5" name="Versión" dataDxfId="57"/>
+    <tableColumn id="6" name="Procesador" dataDxfId="56"/>
+    <tableColumn id="7" name="Utilidad" dataDxfId="55"/>
+    <tableColumn id="8" name="Equipo" dataDxfId="54"/>
+    <tableColumn id="9" name="Contrato privado" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla14" displayName="Tabla14" ref="A17:H22" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla14" displayName="Tabla14" ref="A17:H22" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="A17:H22"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Equipos" dataDxfId="51"/>
-    <tableColumn id="2" name="Fabricante" dataDxfId="50"/>
-    <tableColumn id="3" name="Disponibilidad" dataDxfId="0"/>
-    <tableColumn id="5" name="Versión" dataDxfId="49"/>
-    <tableColumn id="6" name="Procesador" dataDxfId="48"/>
-    <tableColumn id="7" name="Utilidad" dataDxfId="47"/>
-    <tableColumn id="8" name="Equipo" dataDxfId="46"/>
-    <tableColumn id="9" name="Replica Tambo 1" dataDxfId="45"/>
+    <tableColumn id="1" name="Equipos" dataDxfId="50"/>
+    <tableColumn id="2" name="Fabricante" dataDxfId="49"/>
+    <tableColumn id="3" name="Disponibilidad" dataDxfId="48"/>
+    <tableColumn id="5" name="Versión" dataDxfId="47"/>
+    <tableColumn id="6" name="Procesador" dataDxfId="46"/>
+    <tableColumn id="7" name="Utilidad" dataDxfId="45"/>
+    <tableColumn id="8" name="Equipo" dataDxfId="44"/>
+    <tableColumn id="9" name="Replica Tambo 1" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla7" displayName="Tabla7" ref="A2:D35" totalsRowCount="1" headerRowDxfId="44" dataDxfId="43" headerRowCellStyle="Millares" dataCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla7" displayName="Tabla7" ref="A2:D35" totalsRowCount="1" headerRowDxfId="42" dataDxfId="41" headerRowCellStyle="Millares" dataCellStyle="Millares">
   <autoFilter ref="A2:D34"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Producto" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="2" name="Precio Unitario" dataDxfId="40" totalsRowDxfId="39" dataCellStyle="Millares"/>
-    <tableColumn id="3" name="Cantidad" dataDxfId="38" totalsRowDxfId="37" dataCellStyle="Millares"/>
-    <tableColumn id="4" name="Importe" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35" dataCellStyle="Millares">
+    <tableColumn id="1" name="Producto" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="2" name="Precio Unitario" dataDxfId="38" totalsRowDxfId="37" dataCellStyle="Millares"/>
+    <tableColumn id="3" name="Cantidad" dataDxfId="36" totalsRowDxfId="35" dataCellStyle="Millares"/>
+    <tableColumn id="4" name="Importe" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="33" dataCellStyle="Millares">
       <calculatedColumnFormula>+C3*B3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3164,13 +3164,13 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla8" displayName="Tabla8" ref="A2:D23" totalsRowCount="1" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" headerRowCellStyle="Millares" dataCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla8" displayName="Tabla8" ref="A2:D23" totalsRowCount="1" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" headerRowCellStyle="Millares" dataCellStyle="Millares">
   <autoFilter ref="A2:D22"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Producto" dataDxfId="30" totalsRowDxfId="29"/>
-    <tableColumn id="2" name="Precio Unitario" dataDxfId="28" totalsRowDxfId="27" dataCellStyle="Millares"/>
-    <tableColumn id="3" name="Cantidad" dataDxfId="26" totalsRowDxfId="25" dataCellStyle="Millares"/>
-    <tableColumn id="4" name="Importe" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="23" dataCellStyle="Millares">
+    <tableColumn id="1" name="Producto" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="2" name="Precio Unitario" dataDxfId="26" totalsRowDxfId="25" dataCellStyle="Millares"/>
+    <tableColumn id="3" name="Cantidad" dataDxfId="24" totalsRowDxfId="23" dataCellStyle="Millares"/>
+    <tableColumn id="4" name="Importe" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="21" dataCellStyle="Millares">
       <calculatedColumnFormula>+B3*C3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3179,13 +3179,13 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="A2:D26" totalsRowCount="1" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20" headerRowCellStyle="Millares" dataCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="A2:D26" totalsRowCount="1" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18" headerRowCellStyle="Millares" dataCellStyle="Millares">
   <autoFilter ref="A2:D25"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Producto" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="2" name="Precio Unitario" dataDxfId="17" totalsRowDxfId="16" dataCellStyle="Millares"/>
-    <tableColumn id="3" name="Cantidad" dataDxfId="15" totalsRowDxfId="14" dataCellStyle="Millares"/>
-    <tableColumn id="4" name="Importe" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12" dataCellStyle="Millares">
+    <tableColumn id="1" name="Producto" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="2" name="Precio Unitario" dataDxfId="15" totalsRowDxfId="14" dataCellStyle="Millares"/>
+    <tableColumn id="3" name="Cantidad" dataDxfId="13" totalsRowDxfId="12" dataCellStyle="Millares"/>
+    <tableColumn id="4" name="Importe" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10" dataCellStyle="Millares">
       <calculatedColumnFormula>+B3*C3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3194,13 +3194,13 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="A2:D26" totalsRowCount="1" headerRowDxfId="11" dataDxfId="10" headerRowCellStyle="Millares" dataCellStyle="Millares">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="A2:D26" totalsRowCount="1" headerRowDxfId="9" dataDxfId="8" headerRowCellStyle="Millares" dataCellStyle="Millares">
   <autoFilter ref="A2:D25"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Anexos Técnicos" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="2" name="Precio Unitario" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Millares"/>
-    <tableColumn id="3" name="Cantidad" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Millares"/>
-    <tableColumn id="4" name="Importe" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2" dataCellStyle="Millares">
+    <tableColumn id="1" name="Anexos Técnicos" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" name="Precio Unitario" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Millares"/>
+    <tableColumn id="3" name="Cantidad" dataDxfId="3" totalsRowDxfId="2" dataCellStyle="Millares"/>
+    <tableColumn id="4" name="Importe" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Millares">
       <calculatedColumnFormula>+B3*C3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3476,7 +3476,7 @@
   </sheetPr>
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
@@ -5783,7 +5783,7 @@
   </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>

</xml_diff>